<commit_message>
building our own strategy tables
</commit_message>
<xml_diff>
--- a/Strategy1.xlsx
+++ b/Strategy1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonatan\Desktop\21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDF2217-71CA-452F-A983-407D0C52B54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FA01B8-ED5F-49E4-97B8-DADB313FA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,9 +221,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1881,8 +1878,8 @@
   </sheetPr>
   <dimension ref="G1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="68" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3193,7 +3190,7 @@
   </sheetPr>
   <dimension ref="G4:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4:Q41"/>
     </sheetView>
   </sheetViews>
@@ -5487,7 +5484,7 @@
       <c r="K33" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="L33" s="8" t="s">
         <v>2</v>
       </c>
       <c r="M33" s="8" t="s">
@@ -11002,8 +10999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F0259D-EBF3-4A64-A7CB-5AABF0CB47F3}">
   <dimension ref="G4:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:Q41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>